<commit_message>
suzhou - xuhou tickets.
</commit_message>
<xml_diff>
--- a/Chap_05-Achieve/suzhou-xuzhou-tickets.xlsx
+++ b/Chap_05-Achieve/suzhou-xuzhou-tickets.xlsx
@@ -118,7 +118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,6 +128,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -279,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -291,36 +297,16 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -642,7 +628,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D20"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,7 +711,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
+      <c r="A6" s="11">
         <v>0.37986111111111115</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -740,7 +726,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
+      <c r="A7" s="11">
         <v>0.38958333333333334</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -755,7 +741,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+      <c r="A8" s="11">
         <v>0.41250000000000003</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -770,7 +756,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
+      <c r="A9" s="11">
         <v>0.41597222222222219</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -785,7 +771,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
+      <c r="A10" s="11">
         <v>0.41944444444444445</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -800,7 +786,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+      <c r="A11" s="11">
         <v>0.45902777777777781</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -961,13 +947,13 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"常州北"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"无锡东"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"镇江南"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>